<commit_message>
Modified the tailwind screen sizes
</commit_message>
<xml_diff>
--- a/spa/src/Orders/components/Book2.xlsx
+++ b/spa/src/Orders/components/Book2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\api\aron\spa\src\Orders\components\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7FB72A0D-13FF-4089-B909-40A2C8C15649}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{502412DE-F193-44C1-A443-3503119FB5D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1BF52EF5-AA94-41C6-9AE2-C7B10A1D0271}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{1BF52EF5-AA94-41C6-9AE2-C7B10A1D0271}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,41 +37,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="61">
-  <si>
-    <t>discount</t>
-  </si>
-  <si>
-    <t>tax</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="72">
   <si>
     <t>total</t>
   </si>
   <si>
-    <t>with discount</t>
-  </si>
-  <si>
-    <t>before discount</t>
-  </si>
-  <si>
     <t>item tax</t>
   </si>
   <si>
     <t>item price</t>
   </si>
   <si>
-    <t>item 3</t>
-  </si>
-  <si>
-    <t>item 4</t>
-  </si>
-  <si>
-    <t>item 5</t>
-  </si>
-  <si>
-    <t>item 6</t>
-  </si>
-  <si>
     <t>Description</t>
   </si>
   <si>
@@ -220,6 +196,63 @@
   </si>
   <si>
     <t>only</t>
+  </si>
+  <si>
+    <t>eachItem</t>
+  </si>
+  <si>
+    <t>itemDiscount</t>
+  </si>
+  <si>
+    <t>discountShare</t>
+  </si>
+  <si>
+    <t>in the order</t>
+  </si>
+  <si>
+    <t>item level</t>
+  </si>
+  <si>
+    <t>totalItemDiscount</t>
+  </si>
+  <si>
+    <t>activeITem</t>
+  </si>
+  <si>
+    <t>basedOnTotal</t>
+  </si>
+  <si>
+    <t>steps to get total per item</t>
+  </si>
+  <si>
+    <t>get percent of each item in total</t>
+  </si>
+  <si>
+    <t>multiply discount by percentage of item</t>
+  </si>
+  <si>
+    <t>get item total with discount + item discount</t>
+  </si>
+  <si>
+    <t xml:space="preserve">calculate tax for item and add to total item </t>
+  </si>
+  <si>
+    <t>get item total</t>
+  </si>
+  <si>
+    <t>get order total after all calculations</t>
+  </si>
+  <si>
+    <t>product 3</t>
+  </si>
+  <si>
+    <t>product 4</t>
+  </si>
+  <si>
+    <t>product 5</t>
+  </si>
+  <si>
+    <t>product 6</t>
   </si>
 </sst>
 </file>
@@ -306,7 +339,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -380,11 +413,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -418,6 +462,9 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -732,407 +779,457 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{190D4BA0-BBAD-4E11-833E-200CD6DC8F7B}">
-  <dimension ref="A12:O35"/>
+  <dimension ref="A1:L22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" customWidth="1"/>
+    <col min="5" max="5" width="12" customWidth="1"/>
     <col min="6" max="6" width="25.7109375" customWidth="1"/>
-    <col min="8" max="8" width="10.85546875" customWidth="1"/>
-    <col min="9" max="9" width="12.42578125" customWidth="1"/>
+    <col min="7" max="7" width="9.28515625" customWidth="1"/>
+    <col min="8" max="8" width="14.28515625" customWidth="1"/>
+    <col min="9" max="9" width="18.140625" customWidth="1"/>
     <col min="10" max="10" width="15" customWidth="1"/>
     <col min="11" max="11" width="11.140625" customWidth="1"/>
+    <col min="12" max="12" width="28.85546875" customWidth="1"/>
     <col min="14" max="14" width="12.7109375" customWidth="1"/>
     <col min="15" max="15" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="12" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="F12" t="s">
+    <row r="1" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="G12">
-        <v>90000</v>
-      </c>
-    </row>
-    <row r="13" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="F13" t="s">
-        <v>0</v>
-      </c>
-      <c r="G13">
-        <v>4500</v>
-      </c>
-    </row>
-    <row r="14" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="F14" t="s">
+      <c r="D1" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="J1" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="K1" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="L1" s="21" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="11">
         <v>1</v>
       </c>
-      <c r="G14">
-        <v>4500</v>
-      </c>
-    </row>
-    <row r="15" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="F15" t="s">
+      <c r="B2" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="12">
+        <v>3000</v>
+      </c>
+      <c r="D2" s="12">
+        <v>2</v>
+      </c>
+      <c r="E2" s="12">
+        <f>C2*D2</f>
+        <v>6000</v>
+      </c>
+      <c r="F2" s="12">
+        <f>E2/E9*100</f>
+        <v>14.906832298136646</v>
+      </c>
+      <c r="G2" s="11">
+        <f>F2*E11/100</f>
+        <v>300</v>
+      </c>
+      <c r="H2" s="11">
+        <f>E2-G2</f>
+        <v>5700</v>
+      </c>
+      <c r="I2" s="11">
+        <v>0.05</v>
+      </c>
+      <c r="J2" s="11">
+        <f>I2*H2</f>
+        <v>285</v>
+      </c>
+      <c r="K2" s="11">
+        <f>H2+J2</f>
+        <v>5985</v>
+      </c>
+      <c r="L2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="11">
+        <v>2</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="12">
+        <v>2750</v>
+      </c>
+      <c r="D3" s="12">
+        <v>5</v>
+      </c>
+      <c r="E3" s="12">
+        <f t="shared" ref="E3:E7" si="0">C3*D3</f>
+        <v>13750</v>
+      </c>
+      <c r="F3" s="12">
+        <f>E3/E9*100</f>
+        <v>34.161490683229815</v>
+      </c>
+      <c r="G3" s="11">
+        <f>F3*E11/100</f>
+        <v>687.5</v>
+      </c>
+      <c r="H3" s="11">
+        <f t="shared" ref="H3:H7" si="1">E3-G3</f>
+        <v>13062.5</v>
+      </c>
+      <c r="I3" s="11">
+        <v>0.05</v>
+      </c>
+      <c r="J3" s="11">
+        <f t="shared" ref="J3:J7" si="2">I3*H3</f>
+        <v>653.125</v>
+      </c>
+      <c r="K3" s="11">
+        <f t="shared" ref="K3:K7" si="3">H3+J3</f>
+        <v>13715.625</v>
+      </c>
+      <c r="L3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="11">
         <v>3</v>
       </c>
-      <c r="G15">
-        <f>G12-G13</f>
-        <v>85500</v>
-      </c>
-    </row>
-    <row r="16" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="B4" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="C4" s="12">
+        <v>6250</v>
+      </c>
+      <c r="D4" s="12">
+        <v>1</v>
+      </c>
+      <c r="E4" s="12">
+        <f t="shared" si="0"/>
+        <v>6250</v>
+      </c>
+      <c r="F4" s="12">
+        <f>E4/E9*100</f>
+        <v>15.527950310559005</v>
+      </c>
+      <c r="G4" s="11">
+        <f>F4*E11/100</f>
+        <v>312.49999999999994</v>
+      </c>
+      <c r="H4" s="11">
+        <f t="shared" si="1"/>
+        <v>5937.5</v>
+      </c>
+      <c r="I4" s="11">
+        <v>0.05</v>
+      </c>
+      <c r="J4" s="11">
+        <f t="shared" si="2"/>
+        <v>296.875</v>
+      </c>
+      <c r="K4" s="11">
+        <f t="shared" si="3"/>
+        <v>6234.375</v>
+      </c>
+      <c r="L4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="11">
+        <v>4</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="C5" s="12">
+        <v>2000</v>
+      </c>
+      <c r="D5" s="12">
+        <v>6</v>
+      </c>
+      <c r="E5" s="12">
+        <f t="shared" si="0"/>
+        <v>12000</v>
+      </c>
+      <c r="F5" s="12">
+        <f>E5/E9*100</f>
+        <v>29.813664596273291</v>
+      </c>
+      <c r="G5" s="11">
+        <f>F5*E11/100</f>
+        <v>600</v>
+      </c>
+      <c r="H5" s="11">
+        <f t="shared" si="1"/>
+        <v>11400</v>
+      </c>
+      <c r="I5" s="11">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="J5" s="11">
+        <f t="shared" si="2"/>
+        <v>798.00000000000011</v>
+      </c>
+      <c r="K5" s="11">
+        <f t="shared" si="3"/>
+        <v>12198</v>
+      </c>
+      <c r="L5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="11">
+        <v>5</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="C6" s="12">
+        <v>500</v>
+      </c>
+      <c r="D6" s="12">
+        <v>2</v>
+      </c>
+      <c r="E6" s="12">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+      <c r="F6" s="12">
+        <f>E6/E9*100</f>
+        <v>2.4844720496894408</v>
+      </c>
+      <c r="G6" s="11">
+        <f>F6*E11/100</f>
+        <v>50</v>
+      </c>
+      <c r="H6" s="11">
+        <f t="shared" si="1"/>
+        <v>950</v>
+      </c>
+      <c r="I6" s="11">
+        <v>0.1</v>
+      </c>
+      <c r="J6" s="11">
+        <f t="shared" si="2"/>
+        <v>95</v>
+      </c>
+      <c r="K6" s="11">
+        <f t="shared" si="3"/>
+        <v>1045</v>
+      </c>
+      <c r="L6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="11">
+        <v>6</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="C7" s="12">
+        <v>1250</v>
+      </c>
+      <c r="D7" s="12">
+        <v>1</v>
+      </c>
+      <c r="E7" s="12">
+        <f t="shared" si="0"/>
+        <v>1250</v>
+      </c>
+      <c r="F7" s="12">
+        <f>E7/E9*100</f>
+        <v>3.1055900621118013</v>
+      </c>
+      <c r="G7" s="11">
+        <f>F7*E11/100</f>
+        <v>62.5</v>
+      </c>
+      <c r="H7" s="11">
+        <f t="shared" si="1"/>
+        <v>1187.5</v>
+      </c>
+      <c r="I7" s="11">
+        <v>0.05</v>
+      </c>
+      <c r="J7" s="11">
+        <f t="shared" si="2"/>
+        <v>59.375</v>
+      </c>
+      <c r="K7" s="11">
+        <f t="shared" si="3"/>
+        <v>1246.875</v>
+      </c>
+      <c r="L7" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="G8" s="11">
+        <f>SUM(G2:G7)</f>
+        <v>2012.5</v>
+      </c>
+      <c r="H8" s="19">
+        <f>SUM(H2:H7)</f>
+        <v>38237.5</v>
+      </c>
+      <c r="I8" s="11"/>
+      <c r="J8" s="20">
+        <f>SUM(J2:J7)</f>
+        <v>2187.375</v>
+      </c>
+      <c r="K8" s="18">
+        <f>SUM(K2:K7)</f>
+        <v>40424.875</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" s="3">
+        <f>SUM(E2:E8)</f>
+        <v>40250</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D10" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" s="5">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D11" s="6"/>
+      <c r="E11" s="5">
+        <f>E9*E10</f>
+        <v>2012.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D12" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" s="8">
+        <f>E9-E11</f>
+        <v>38237.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D13" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E13" s="10">
+        <f>J8</f>
+        <v>2187.375</v>
+      </c>
+      <c r="H13" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D14" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="E14" s="18">
+        <f>E12+E13</f>
+        <v>40424.875</v>
+      </c>
+      <c r="H14" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H15" t="s">
+        <v>53</v>
+      </c>
+      <c r="I15" t="s">
+        <v>54</v>
+      </c>
+      <c r="J15" t="s">
+        <v>57</v>
+      </c>
+      <c r="K15" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D16">
         <v>0.5</v>
       </c>
       <c r="F16" t="s">
+        <v>0</v>
+      </c>
+      <c r="G16" t="e">
+        <f>#REF!+#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="I16" t="s">
+        <v>55</v>
+      </c>
+      <c r="J16" t="s">
+        <v>56</v>
+      </c>
+      <c r="K16" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
         <v>2</v>
       </c>
-      <c r="G16">
-        <f>G15+G14</f>
-        <v>90000</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C17" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15" ht="60" x14ac:dyDescent="0.25">
+      <c r="I17" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="E22" t="s">
-        <v>25</v>
-      </c>
-      <c r="F22" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="G22" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="H22" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="I22" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="J22" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="K22" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="L22" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="M22" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="N22" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="O22" s="15" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="F23" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="G23" s="12">
-        <v>3000</v>
-      </c>
-      <c r="H23" s="12">
-        <v>2</v>
-      </c>
-      <c r="I23" s="12">
-        <f>G23*H23</f>
-        <v>6000</v>
-      </c>
-      <c r="J23" s="12">
-        <f>I23/I30*100</f>
-        <v>14.906832298136646</v>
-      </c>
-      <c r="K23" s="11">
-        <f>J23*I32/100</f>
-        <v>600</v>
-      </c>
-      <c r="L23" s="11">
-        <f>I23-K23</f>
-        <v>5400</v>
-      </c>
-      <c r="M23" s="11">
-        <v>0.05</v>
-      </c>
-      <c r="N23" s="11">
-        <f>M23*L23</f>
-        <v>270</v>
-      </c>
-      <c r="O23" s="11">
-        <f>L23+N23</f>
-        <v>5670</v>
-      </c>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="F24" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="G24" s="12">
-        <v>2750</v>
-      </c>
-      <c r="H24" s="12">
-        <v>5</v>
-      </c>
-      <c r="I24" s="12">
-        <f t="shared" ref="I24:I28" si="0">G24*H24</f>
-        <v>13750</v>
-      </c>
-      <c r="J24" s="12">
-        <f>I24/I30*100</f>
-        <v>34.161490683229815</v>
-      </c>
-      <c r="K24" s="11">
-        <f>J24*I32/100</f>
-        <v>1375</v>
-      </c>
-      <c r="L24" s="11">
-        <f t="shared" ref="L24:L28" si="1">I24-K24</f>
-        <v>12375</v>
-      </c>
-      <c r="M24" s="11">
-        <v>0.05</v>
-      </c>
-      <c r="N24" s="11">
-        <f t="shared" ref="N24:N28" si="2">M24*L24</f>
-        <v>618.75</v>
-      </c>
-      <c r="O24" s="11">
-        <f t="shared" ref="O24:O28" si="3">L24+N24</f>
-        <v>12993.75</v>
-      </c>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="F25" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="G25" s="12">
-        <v>6250</v>
-      </c>
-      <c r="H25" s="12">
-        <v>1</v>
-      </c>
-      <c r="I25" s="12">
-        <f t="shared" si="0"/>
-        <v>6250</v>
-      </c>
-      <c r="J25" s="12">
-        <f>I25/I30*100</f>
-        <v>15.527950310559005</v>
-      </c>
-      <c r="K25" s="11">
-        <f>J25*I32/100</f>
-        <v>624.99999999999989</v>
-      </c>
-      <c r="L25" s="11">
-        <f t="shared" si="1"/>
-        <v>5625</v>
-      </c>
-      <c r="M25" s="11">
-        <v>0.05</v>
-      </c>
-      <c r="N25" s="11">
-        <f t="shared" si="2"/>
-        <v>281.25</v>
-      </c>
-      <c r="O25" s="11">
-        <f t="shared" si="3"/>
-        <v>5906.25</v>
-      </c>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="F26" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="G26" s="12">
-        <v>2000</v>
-      </c>
-      <c r="H26" s="12">
-        <v>6</v>
-      </c>
-      <c r="I26" s="12">
-        <f t="shared" si="0"/>
-        <v>12000</v>
-      </c>
-      <c r="J26" s="12">
-        <f>I26/I30*100</f>
-        <v>29.813664596273291</v>
-      </c>
-      <c r="K26" s="11">
-        <f>J26*I32/100</f>
-        <v>1200</v>
-      </c>
-      <c r="L26" s="11">
-        <f t="shared" si="1"/>
-        <v>10800</v>
-      </c>
-      <c r="M26" s="11">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="N26" s="11">
-        <f t="shared" si="2"/>
-        <v>756.00000000000011</v>
-      </c>
-      <c r="O26" s="11">
-        <f t="shared" si="3"/>
-        <v>11556</v>
-      </c>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="F27" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="G27" s="12">
-        <v>500</v>
-      </c>
-      <c r="H27" s="12">
-        <v>2</v>
-      </c>
-      <c r="I27" s="12">
-        <f t="shared" si="0"/>
-        <v>1000</v>
-      </c>
-      <c r="J27" s="12">
-        <f>I27/I30*100</f>
-        <v>2.4844720496894408</v>
-      </c>
-      <c r="K27" s="11">
-        <f>J27*I32/100</f>
-        <v>100</v>
-      </c>
-      <c r="L27" s="11">
-        <f t="shared" si="1"/>
-        <v>900</v>
-      </c>
-      <c r="M27" s="11">
-        <v>0.1</v>
-      </c>
-      <c r="N27" s="11">
-        <f t="shared" si="2"/>
-        <v>90</v>
-      </c>
-      <c r="O27" s="11">
-        <f t="shared" si="3"/>
-        <v>990</v>
-      </c>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="F28" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="G28" s="12">
-        <v>1250</v>
-      </c>
-      <c r="H28" s="12">
-        <v>1</v>
-      </c>
-      <c r="I28" s="12">
-        <f t="shared" si="0"/>
-        <v>1250</v>
-      </c>
-      <c r="J28" s="12">
-        <f>I28/I30*100</f>
-        <v>3.1055900621118013</v>
-      </c>
-      <c r="K28" s="11">
-        <f>J28*I32/100</f>
-        <v>125</v>
-      </c>
-      <c r="L28" s="11">
-        <f t="shared" si="1"/>
-        <v>1125</v>
-      </c>
-      <c r="M28" s="11">
-        <v>0.05</v>
-      </c>
-      <c r="N28" s="11">
-        <f t="shared" si="2"/>
-        <v>56.25</v>
-      </c>
-      <c r="O28" s="11">
-        <f t="shared" si="3"/>
-        <v>1181.25</v>
-      </c>
-    </row>
-    <row r="29" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="K29" s="11">
-        <f>SUM(K23:K28)</f>
-        <v>4025</v>
-      </c>
-      <c r="L29" s="19">
-        <f>SUM(L23:L28)</f>
-        <v>36225</v>
-      </c>
-      <c r="M29" s="11"/>
-      <c r="N29" s="20">
-        <f>SUM(N23:N28)</f>
-        <v>2072.25</v>
-      </c>
-      <c r="O29" s="18">
-        <f>SUM(O23:O28)</f>
-        <v>38297.25</v>
-      </c>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="H30" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I30" s="3">
-        <f>SUM(I23:I29)</f>
-        <v>40250</v>
-      </c>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="H31" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="I31" s="5">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="H32" s="6"/>
-      <c r="I32" s="5">
-        <f>I30*I31</f>
-        <v>4025</v>
-      </c>
-    </row>
-    <row r="33" spans="8:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="H33" s="7" t="s">
         <v>17</v>
-      </c>
-      <c r="I33" s="8">
-        <f>I30-I32</f>
-        <v>36225</v>
-      </c>
-    </row>
-    <row r="34" spans="8:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="H34" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="I34" s="10">
-        <v>2072.25</v>
-      </c>
-    </row>
-    <row r="35" spans="8:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="H35" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="I35" s="18">
-        <f>I33+I34</f>
-        <v>38297.25</v>
       </c>
     </row>
   </sheetData>
@@ -1157,146 +1254,146 @@
   <sheetData>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="D3" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="F3" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="D8" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="E8" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="D9" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="G9" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D10" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="E10" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="G10" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="H10" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="I10" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D11" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="E11" t="s">
+        <v>34</v>
+      </c>
+      <c r="G11" t="s">
         <v>42</v>
-      </c>
-      <c r="G11" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D12" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D13" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="E13" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D14" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="E14" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D15" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="E15" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
     </row>
     <row r="17" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D17" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
     </row>
     <row r="18" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D18" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
     </row>
     <row r="19" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D19" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
     </row>
     <row r="20" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D20" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
     </row>
     <row r="21" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D21" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="E21" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
     </row>
     <row r="22" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D22" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="E22" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
     </row>
     <row r="23" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D23" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="E23" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Still working on calculations of total with tax
</commit_message>
<xml_diff>
--- a/spa/src/Orders/components/Book2.xlsx
+++ b/spa/src/Orders/components/Book2.xlsx
@@ -5,16 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\api\aron\spa\src\Orders\components\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\api\aron\spa\src\Orders\components\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{266FB0A2-A607-4F1E-8ED9-ED742603A1C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21DE7F1F-2415-4339-A0F5-77633B7B163B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1BF52EF5-AA94-41C6-9AE2-C7B10A1D0271}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{1BF52EF5-AA94-41C6-9AE2-C7B10A1D0271}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -24,12 +25,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -37,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="80">
   <si>
     <t>total</t>
   </si>
@@ -253,6 +251,30 @@
   </si>
   <si>
     <t>product 6</t>
+  </si>
+  <si>
+    <t>Tic Quality Control</t>
+  </si>
+  <si>
+    <t>company name</t>
+  </si>
+  <si>
+    <t>Adress</t>
+  </si>
+  <si>
+    <t>calculateOrderDiscount</t>
+  </si>
+  <si>
+    <t>itemPercent</t>
+  </si>
+  <si>
+    <t>itemTotal /itemsTotal</t>
+  </si>
+  <si>
+    <t>orderDiscount/100 or orderDiscount</t>
+  </si>
+  <si>
+    <t>itemDiscount + itemPercent * calculateOrderDiscount</t>
   </si>
 </sst>
 </file>
@@ -781,8 +803,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{190D4BA0-BBAD-4E11-833E-200CD6DC8F7B}">
   <dimension ref="A1:L22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F20" sqref="F20:G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1239,6 +1261,62 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72FBAB34-766B-4CE9-B582-89F781464C8F}">
+  <dimension ref="C4:D9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="31" customWidth="1"/>
+    <col min="4" max="4" width="43.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>73</v>
+      </c>
+      <c r="D4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="5" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="7" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>76</v>
+      </c>
+      <c r="D7" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="8" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>75</v>
+      </c>
+      <c r="D8" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="9" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>54</v>
+      </c>
+      <c r="D9" t="s">
+        <v>79</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50429D35-DF85-4406-AE94-16F108B60830}">
   <dimension ref="A2:I23"/>
   <sheetViews>

</xml_diff>

<commit_message>
First order submitted, need to make documents...
</commit_message>
<xml_diff>
--- a/spa/src/Orders/components/Book2.xlsx
+++ b/spa/src/Orders/components/Book2.xlsx
@@ -5,17 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\api\aron\spa\src\Orders\components\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\api\aron\spa\src\Orders\components\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21DE7F1F-2415-4339-A0F5-77633B7B163B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F45C6B82-894B-4D0E-973F-DA6CF3EBDBAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{1BF52EF5-AA94-41C6-9AE2-C7B10A1D0271}"/>
+    <workbookView xWindow="7620" yWindow="630" windowWidth="15330" windowHeight="10920" activeTab="1" xr2:uid="{1BF52EF5-AA94-41C6-9AE2-C7B10A1D0271}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
+    <sheet name="OrderPayload" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,9 +26,12 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -35,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="90">
   <si>
     <t>total</t>
   </si>
@@ -275,6 +279,36 @@
   </si>
   <si>
     <t>itemDiscount + itemPercent * calculateOrderDiscount</t>
+  </si>
+  <si>
+    <t>Order Payload</t>
+  </si>
+  <si>
+    <t>onSubmit</t>
+  </si>
+  <si>
+    <t>Management</t>
+  </si>
+  <si>
+    <t>Documents</t>
+  </si>
+  <si>
+    <t>Stock</t>
+  </si>
+  <si>
+    <t>Reposrting</t>
+  </si>
+  <si>
+    <t>Customers &amp; suppliers</t>
+  </si>
+  <si>
+    <t>Promotions &amp; actions</t>
+  </si>
+  <si>
+    <t>Users &amp; security</t>
+  </si>
+  <si>
+    <t>Cash Registers</t>
   </si>
 </sst>
 </file>
@@ -1262,10 +1296,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72FBAB34-766B-4CE9-B582-89F781464C8F}">
-  <dimension ref="C4:D9"/>
+  <dimension ref="C4:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1309,6 +1343,56 @@
       </c>
       <c r="D9" t="s">
         <v>79</v>
+      </c>
+    </row>
+    <row r="13" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="14" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="16" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="18" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="19" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="20" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="21" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="22" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -1477,4 +1561,31 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B562DA3-F9A5-4CAC-ABB3-2D80BE9C4F4B}">
+  <dimension ref="C5:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="16.85546875" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="5" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>80</v>
+      </c>
+      <c r="D5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added some excel markdowns
</commit_message>
<xml_diff>
--- a/spa/src/Orders/components/Book2.xlsx
+++ b/spa/src/Orders/components/Book2.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\api\aron\spa\src\Orders\components\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F45C6B82-894B-4D0E-973F-DA6CF3EBDBAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A3E6BDC-0830-4694-8F43-694355C4CD33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7620" yWindow="630" windowWidth="15330" windowHeight="10920" activeTab="1" xr2:uid="{1BF52EF5-AA94-41C6-9AE2-C7B10A1D0271}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{1BF52EF5-AA94-41C6-9AE2-C7B10A1D0271}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
-    <sheet name="OrderPayload" sheetId="4" r:id="rId4"/>
+    <sheet name="Layout" sheetId="5" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId4"/>
+    <sheet name="OrderPayload" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="109">
   <si>
     <t>total</t>
   </si>
@@ -309,6 +310,63 @@
   </si>
   <si>
     <t>Cash Registers</t>
+  </si>
+  <si>
+    <t>Server</t>
+  </si>
+  <si>
+    <t>Client</t>
+  </si>
+  <si>
+    <t>API for Fetch Data</t>
+  </si>
+  <si>
+    <t>Web Application</t>
+  </si>
+  <si>
+    <t>User creation</t>
+  </si>
+  <si>
+    <t>Store Front</t>
+  </si>
+  <si>
+    <t>Add Items, sell items</t>
+  </si>
+  <si>
+    <t>Create and submit orders</t>
+  </si>
+  <si>
+    <t>Close cash register</t>
+  </si>
+  <si>
+    <t>create report related to cash register based on user level</t>
+  </si>
+  <si>
+    <t>control user interface</t>
+  </si>
+  <si>
+    <t>app settings like colors and language</t>
+  </si>
+  <si>
+    <t>Stocks</t>
+  </si>
+  <si>
+    <t>Printers</t>
+  </si>
+  <si>
+    <t>setting up print stations</t>
+  </si>
+  <si>
+    <t>Create and manage users</t>
+  </si>
+  <si>
+    <t>Permissions and authorizations</t>
+  </si>
+  <si>
+    <t>Like the store</t>
+  </si>
+  <si>
+    <t>create and submit orders</t>
   </si>
 </sst>
 </file>
@@ -1298,7 +1356,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72FBAB34-766B-4CE9-B582-89F781464C8F}">
   <dimension ref="C4:D22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
@@ -1401,6 +1459,114 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E44F39B-5607-4D35-9E1A-8744D393F2A2}">
+  <dimension ref="B3:M11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="21.28515625" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>90</v>
+      </c>
+      <c r="M3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="4" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="M4" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>92</v>
+      </c>
+      <c r="M5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="6" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>93</v>
+      </c>
+      <c r="C6" t="s">
+        <v>107</v>
+      </c>
+      <c r="E6" t="s">
+        <v>108</v>
+      </c>
+      <c r="M6" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>82</v>
+      </c>
+      <c r="C7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" t="s">
+        <v>83</v>
+      </c>
+      <c r="E7" t="s">
+        <v>38</v>
+      </c>
+      <c r="F7" t="s">
+        <v>102</v>
+      </c>
+      <c r="G7" t="s">
+        <v>103</v>
+      </c>
+      <c r="M7" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="8" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C8" t="s">
+        <v>105</v>
+      </c>
+      <c r="E8" t="s">
+        <v>106</v>
+      </c>
+      <c r="M8" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="9" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="M9" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="M10" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="M11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50429D35-DF85-4406-AE94-16F108B60830}">
   <dimension ref="A2:I23"/>
   <sheetViews>
@@ -1563,7 +1729,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B562DA3-F9A5-4CAC-ABB3-2D80BE9C4F4B}">
   <dimension ref="C5:D5"/>
   <sheetViews>

</xml_diff>